<commit_message>
add report data save function
</commit_message>
<xml_diff>
--- a/src/util/report_items_pandas.xlsx
+++ b/src/util/report_items_pandas.xlsx
@@ -434,20 +434,20 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="6" customWidth="1" min="1" max="1"/>
-    <col width="12" customWidth="1" min="2" max="2"/>
-    <col width="12" customWidth="1" min="3" max="3"/>
-    <col width="6" customWidth="1" min="4" max="4"/>
-    <col width="16" customWidth="1" min="5" max="5"/>
-    <col width="6" customWidth="1" min="6" max="6"/>
-    <col width="7" customWidth="1" min="7" max="7"/>
-    <col width="7" customWidth="1" min="8" max="8"/>
-    <col width="15" customWidth="1" min="9" max="9"/>
-    <col width="12" customWidth="1" min="10" max="10"/>
-    <col width="14" customWidth="1" min="11" max="11"/>
-    <col width="14" customWidth="1" min="12" max="12"/>
-    <col width="11" customWidth="1" min="13" max="13"/>
-    <col width="18" customWidth="1" min="14" max="14"/>
+    <col width="7" customWidth="1" min="1" max="1"/>
+    <col width="7" customWidth="1" min="2" max="2"/>
+    <col width="11" customWidth="1" min="3" max="3"/>
+    <col width="7" customWidth="1" min="4" max="4"/>
+    <col width="8" customWidth="1" min="5" max="5"/>
+    <col width="7" customWidth="1" min="6" max="6"/>
+    <col width="8" customWidth="1" min="7" max="7"/>
+    <col width="8" customWidth="1" min="8" max="8"/>
+    <col width="16" customWidth="1" min="9" max="9"/>
+    <col width="13" customWidth="1" min="10" max="10"/>
+    <col width="15" customWidth="1" min="11" max="11"/>
+    <col width="15" customWidth="1" min="12" max="12"/>
+    <col width="12" customWidth="1" min="13" max="13"/>
+    <col width="19" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -523,27 +523,11 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>ID_1</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2023-05-20</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Category A</t>
-        </is>
-      </c>
+      <c r="A2" t="inlineStr"/>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Report Title 1</t>
-        </is>
-      </c>
+      <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
@@ -555,27 +539,11 @@
       <c r="N2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>ID_2</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2023-05-20</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Category A</t>
-        </is>
-      </c>
+      <c r="A3" t="inlineStr"/>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Report Title 2</t>
-        </is>
-      </c>
+      <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>

</xml_diff>